<commit_message>
Implemented cleanup logic for contacts
</commit_message>
<xml_diff>
--- a/Assets/Template_long_v2.xlsx
+++ b/Assets/Template_long_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\workspace\Regio\Regio.Bexio\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C6F16E-419E-4147-9B50-90856EF0FF4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70EA364-8B56-4F8E-94A5-21731A5A3835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1965" yWindow="1965" windowWidth="18000" windowHeight="12675" xr2:uid="{3AA70410-87DE-4FA9-A71D-D4E551EB54C4}"/>
+    <workbookView xWindow="12000" yWindow="0" windowWidth="12000" windowHeight="17400" xr2:uid="{3AA70410-87DE-4FA9-A71D-D4E551EB54C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -1004,8 +1004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED85B2AD-F9E3-48AB-A87E-0AD8C887EFD8}">
   <dimension ref="A2:S65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2598,7 +2598,7 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>2024036</v>
+        <v>2024136</v>
       </c>
       <c r="B30" s="1">
         <v>46418</v>

</xml_diff>